<commit_message>
data update by heike
</commit_message>
<xml_diff>
--- a/FSP_Exchange/data/Overview_Stat_Analyses.xlsx
+++ b/FSP_Exchange/data/Overview_Stat_Analyses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thermofisher-my.sharepoint.com/personal/heike_goehler_thermofisher_com/Documents/FSP_Exchange/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="402" documentId="8_{B71B119A-91B9-41B4-A31F-26ADBC8182F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C448BCC-77D1-4A33-AA70-CEF039ACCD98}"/>
+  <xr:revisionPtr revIDLastSave="410" documentId="8_{B71B119A-91B9-41B4-A31F-26ADBC8182F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58A02337-A6C5-4DC2-9E22-472E410D2336}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{DB58F8A3-982D-4375-901B-E1B15CF4D99D}"/>
   </bookViews>
@@ -964,7 +964,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1028,8 +1028,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1396,11 +1394,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D59CA7-78DE-483F-8DC5-D261426A3AA3}">
   <dimension ref="A1:AL124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="T3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A35" sqref="A35:XFD35"/>
+      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2071,7 +2069,7 @@
       <c r="Q9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="R9" s="37" t="s">
+      <c r="R9" s="2" t="s">
         <v>37</v>
       </c>
       <c r="S9" s="2" t="s">
@@ -2150,7 +2148,7 @@
       <c r="Q10" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="R10" s="37" t="s">
+      <c r="R10" s="2" t="s">
         <v>37</v>
       </c>
       <c r="S10" s="20" t="s">
@@ -2227,7 +2225,7 @@
       <c r="Q11" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="R11" s="38" t="s">
+      <c r="R11" s="20" t="s">
         <v>37</v>
       </c>
       <c r="S11" s="20" t="s">
@@ -2537,7 +2535,7 @@
       <c r="O15" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="P15" s="39" t="s">
+      <c r="P15" s="37" t="s">
         <v>241</v>
       </c>
       <c r="Q15" s="20" t="s">
@@ -2546,7 +2544,7 @@
       <c r="R15" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="S15" s="38" t="s">
+      <c r="S15" s="20" t="s">
         <v>31</v>
       </c>
       <c r="T15" s="20" t="s">
@@ -2619,7 +2617,7 @@
       <c r="R16" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="S16" s="37" t="s">
+      <c r="S16" s="2" t="s">
         <v>33</v>
       </c>
       <c r="T16" s="20" t="s">
@@ -2768,7 +2766,7 @@
       <c r="O18" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="P18" s="39" t="s">
+      <c r="P18" s="37" t="s">
         <v>241</v>
       </c>
       <c r="Q18" s="20" t="s">

</xml_diff>

<commit_message>
dada entry correction manual
</commit_message>
<xml_diff>
--- a/FSP_Exchange/data/Overview_Stat_Analyses.xlsx
+++ b/FSP_Exchange/data/Overview_Stat_Analyses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thermofisher-my.sharepoint.com/personal/heike_goehler_thermofisher_com/Documents/FSP_Exchange/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefa\OneDrive\Dokumente\Career\Freelance\_Kunden\BRAHMS\2024 - FSP\fsp_validation\FSP_Exchange\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="410" documentId="8_{B71B119A-91B9-41B4-A31F-26ADBC8182F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58A02337-A6C5-4DC2-9E22-472E410D2336}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECA2313-BEC1-4E64-9016-914F5FE7E831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{DB58F8A3-982D-4375-901B-E1B15CF4D99D}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{DB58F8A3-982D-4375-901B-E1B15CF4D99D}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1826" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1827" uniqueCount="244">
   <si>
     <t>Analysis</t>
   </si>
@@ -1031,7 +1031,7 @@
     <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1096,9 +1096,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1136,7 +1136,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1242,7 +1242,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1384,7 +1384,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1395,42 +1395,42 @@
   <dimension ref="A1:AL124"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomRight" activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.7109375" customWidth="1"/>
-    <col min="8" max="8" width="37.28515625" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
-    <col min="12" max="12" width="33.42578125" customWidth="1"/>
-    <col min="13" max="13" width="28.42578125" customWidth="1"/>
-    <col min="14" max="14" width="23.140625" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" customWidth="1"/>
-    <col min="17" max="17" width="21.42578125" customWidth="1"/>
-    <col min="18" max="18" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.42578125" customWidth="1"/>
-    <col min="20" max="20" width="22.7109375" customWidth="1"/>
-    <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.85546875" customWidth="1"/>
-    <col min="23" max="23" width="31.7109375" customWidth="1"/>
-    <col min="24" max="24" width="21.85546875" customWidth="1"/>
-    <col min="25" max="26" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.68359375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="16.26171875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="20.578125" customWidth="1"/>
+    <col min="4" max="4" width="5.578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.41796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.41796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.68359375" customWidth="1"/>
+    <col min="8" max="8" width="37.26171875" customWidth="1"/>
+    <col min="9" max="9" width="10.83984375" customWidth="1"/>
+    <col min="10" max="10" width="12.15625" customWidth="1"/>
+    <col min="11" max="11" width="15.68359375" customWidth="1"/>
+    <col min="12" max="12" width="33.41796875" customWidth="1"/>
+    <col min="13" max="13" width="28.41796875" customWidth="1"/>
+    <col min="14" max="14" width="23.15625" customWidth="1"/>
+    <col min="15" max="15" width="13.41796875" customWidth="1"/>
+    <col min="16" max="16" width="12.68359375" customWidth="1"/>
+    <col min="17" max="17" width="21.41796875" customWidth="1"/>
+    <col min="18" max="18" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.41796875" customWidth="1"/>
+    <col min="20" max="20" width="22.68359375" customWidth="1"/>
+    <col min="21" max="21" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.83984375" customWidth="1"/>
+    <col min="23" max="23" width="31.68359375" customWidth="1"/>
+    <col min="24" max="24" width="21.83984375" customWidth="1"/>
+    <col min="25" max="26" width="21.26171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
@@ -1464,7 +1464,7 @@
       <c r="Y1" s="35"/>
       <c r="Z1" s="35"/>
     </row>
-    <row r="2" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="26" t="s">
         <v>3</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="27">
         <v>45334</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="27">
         <v>45334</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="27">
         <v>45334</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="27">
         <v>45334</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="27">
         <v>45334</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="28">
         <v>45334</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="27">
         <v>45334</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="27">
         <v>45334</v>
       </c>
@@ -2154,7 +2154,9 @@
       <c r="S10" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="T10" s="2"/>
+      <c r="T10" s="20" t="s">
+        <v>31</v>
+      </c>
       <c r="U10" s="31" t="s">
         <v>31</v>
       </c>
@@ -2174,7 +2176,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="27">
         <v>45334</v>
       </c>
@@ -2253,7 +2255,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="28">
         <v>45334</v>
       </c>
@@ -2332,7 +2334,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="27">
         <v>45334</v>
       </c>
@@ -2411,7 +2413,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="27">
         <v>45334</v>
       </c>
@@ -2490,7 +2492,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="27">
         <v>45334</v>
       </c>
@@ -2563,7 +2565,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="27">
         <v>45334</v>
       </c>
@@ -2642,7 +2644,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="27">
         <v>45334</v>
       </c>
@@ -2721,7 +2723,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="27">
         <v>45334</v>
       </c>
@@ -2794,7 +2796,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="28">
         <v>45334</v>
       </c>
@@ -2873,7 +2875,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="27">
         <v>45343</v>
       </c>
@@ -2944,7 +2946,7 @@
       <c r="Y20" s="19"/>
       <c r="Z20" s="19"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="28">
         <v>45343</v>
       </c>
@@ -3015,7 +3017,7 @@
       <c r="Y21" s="15"/>
       <c r="Z21" s="15"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="27">
         <v>45343</v>
       </c>
@@ -3086,7 +3088,7 @@
       <c r="Y22" s="11"/>
       <c r="Z22" s="11"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="27">
         <v>45343</v>
       </c>
@@ -3157,7 +3159,7 @@
       <c r="Y23" s="19"/>
       <c r="Z23" s="19"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="27">
         <v>45343</v>
       </c>
@@ -3228,7 +3230,7 @@
       <c r="Y24" s="19"/>
       <c r="Z24" s="19"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="27">
         <v>45343</v>
       </c>
@@ -3299,7 +3301,7 @@
       <c r="Y25" s="19"/>
       <c r="Z25" s="19"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="27">
         <v>45343</v>
       </c>
@@ -3370,7 +3372,7 @@
       <c r="Y26" s="19"/>
       <c r="Z26" s="19"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="27">
         <v>45343</v>
       </c>
@@ -3439,7 +3441,7 @@
       <c r="Y27" s="19"/>
       <c r="Z27" s="19"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="27">
         <v>45343</v>
       </c>
@@ -3508,7 +3510,7 @@
       <c r="Y28" s="19"/>
       <c r="Z28" s="19"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="27">
         <v>45343</v>
       </c>
@@ -3579,7 +3581,7 @@
       <c r="Y29" s="19"/>
       <c r="Z29" s="19"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="27">
         <v>45343</v>
       </c>
@@ -3650,7 +3652,7 @@
       <c r="Y30" s="19"/>
       <c r="Z30" s="19"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="27">
         <v>45343</v>
       </c>
@@ -3721,7 +3723,7 @@
       <c r="Y31" s="19"/>
       <c r="Z31" s="19"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="27">
         <v>45343</v>
       </c>
@@ -3792,7 +3794,7 @@
       <c r="Y32" s="19"/>
       <c r="Z32" s="19"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="27">
         <v>45343</v>
       </c>
@@ -3863,7 +3865,7 @@
       <c r="Y33" s="19"/>
       <c r="Z33" s="19"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="28">
         <v>45343</v>
       </c>
@@ -3934,7 +3936,7 @@
       <c r="Y34" s="19"/>
       <c r="Z34" s="19"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="27">
         <v>45348</v>
       </c>
@@ -4005,7 +4007,7 @@
       <c r="Y35" s="11"/>
       <c r="Z35" s="11"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="27">
         <v>45348</v>
       </c>
@@ -4076,7 +4078,7 @@
       <c r="Y36" s="19"/>
       <c r="Z36" s="19"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="27">
         <v>45348</v>
       </c>
@@ -4147,7 +4149,7 @@
       <c r="Y37" s="19"/>
       <c r="Z37" s="19"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="27">
         <v>45348</v>
       </c>
@@ -4218,7 +4220,7 @@
       <c r="Y38" s="19"/>
       <c r="Z38" s="19"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="27">
         <v>45348</v>
       </c>
@@ -4289,7 +4291,7 @@
       <c r="Y39" s="19"/>
       <c r="Z39" s="19"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="27">
         <v>45348</v>
       </c>
@@ -4360,7 +4362,7 @@
       <c r="Y40" s="19"/>
       <c r="Z40" s="19"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="27">
         <v>45348</v>
       </c>
@@ -4431,7 +4433,7 @@
       <c r="Y41" s="19"/>
       <c r="Z41" s="19"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="27">
         <v>45348</v>
       </c>
@@ -4502,7 +4504,7 @@
       <c r="Y42" s="19"/>
       <c r="Z42" s="19"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="27">
         <v>45348</v>
       </c>
@@ -4573,7 +4575,7 @@
       <c r="Y43" s="19"/>
       <c r="Z43" s="19"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="27">
         <v>45348</v>
       </c>
@@ -4644,7 +4646,7 @@
       <c r="Y44" s="19"/>
       <c r="Z44" s="19"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="27">
         <v>45348</v>
       </c>
@@ -4715,7 +4717,7 @@
       <c r="Y45" s="19"/>
       <c r="Z45" s="19"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="27">
         <v>45348</v>
       </c>
@@ -4786,7 +4788,7 @@
       <c r="Y46" s="19"/>
       <c r="Z46" s="19"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="27">
         <v>45348</v>
       </c>
@@ -4857,7 +4859,7 @@
       <c r="Y47" s="19"/>
       <c r="Z47" s="19"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="27">
         <v>45348</v>
       </c>
@@ -4928,7 +4930,7 @@
       <c r="Y48" s="19"/>
       <c r="Z48" s="19"/>
     </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="27">
         <v>45348</v>
       </c>
@@ -4999,7 +5001,7 @@
       <c r="Y49" s="19"/>
       <c r="Z49" s="19"/>
     </row>
-    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="27">
         <v>45348</v>
       </c>
@@ -5070,7 +5072,7 @@
       <c r="Y50" s="19"/>
       <c r="Z50" s="19"/>
     </row>
-    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="27">
         <v>45348</v>
       </c>
@@ -5142,7 +5144,7 @@
       <c r="Z51" s="19"/>
       <c r="AL51" s="33"/>
     </row>
-    <row r="52" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="28">
         <v>45348</v>
       </c>
@@ -5214,7 +5216,7 @@
       <c r="Z52" s="19"/>
       <c r="AL52" s="33"/>
     </row>
-    <row r="53" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="27">
         <v>45356</v>
       </c>
@@ -5285,7 +5287,7 @@
       <c r="Y53" s="11"/>
       <c r="Z53" s="11"/>
     </row>
-    <row r="54" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="27">
         <v>45356</v>
       </c>
@@ -5356,7 +5358,7 @@
       <c r="Y54" s="19"/>
       <c r="Z54" s="19"/>
     </row>
-    <row r="55" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="27">
         <v>45356</v>
       </c>
@@ -5427,7 +5429,7 @@
       <c r="Y55" s="19"/>
       <c r="Z55" s="19"/>
     </row>
-    <row r="56" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="27">
         <v>45356</v>
       </c>
@@ -5498,7 +5500,7 @@
       <c r="Y56" s="19"/>
       <c r="Z56" s="19"/>
     </row>
-    <row r="57" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="27">
         <v>45356</v>
       </c>
@@ -5569,7 +5571,7 @@
       <c r="Y57" s="19"/>
       <c r="Z57" s="19"/>
     </row>
-    <row r="58" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="27">
         <v>45356</v>
       </c>
@@ -5640,7 +5642,7 @@
       <c r="Y58" s="19"/>
       <c r="Z58" s="19"/>
     </row>
-    <row r="59" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="27">
         <v>45356</v>
       </c>
@@ -5711,7 +5713,7 @@
       <c r="Y59" s="19"/>
       <c r="Z59" s="19"/>
     </row>
-    <row r="60" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="27">
         <v>45356</v>
       </c>
@@ -5782,7 +5784,7 @@
       <c r="Y60" s="19"/>
       <c r="Z60" s="19"/>
     </row>
-    <row r="61" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="27">
         <v>45356</v>
       </c>
@@ -5853,7 +5855,7 @@
       <c r="Y61" s="19"/>
       <c r="Z61" s="19"/>
     </row>
-    <row r="62" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="27">
         <v>45356</v>
       </c>
@@ -5924,7 +5926,7 @@
       <c r="Y62" s="19"/>
       <c r="Z62" s="19"/>
     </row>
-    <row r="63" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="27">
         <v>45356</v>
       </c>
@@ -5995,7 +5997,7 @@
       <c r="Y63" s="19"/>
       <c r="Z63" s="19"/>
     </row>
-    <row r="64" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="27">
         <v>45356</v>
       </c>
@@ -6066,7 +6068,7 @@
       <c r="Y64" s="19"/>
       <c r="Z64" s="19"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="27">
         <v>45356</v>
       </c>
@@ -6137,7 +6139,7 @@
       <c r="Y65" s="19"/>
       <c r="Z65" s="19"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="27">
         <v>45356</v>
       </c>
@@ -6208,7 +6210,7 @@
       <c r="Y66" s="19"/>
       <c r="Z66" s="19"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="27">
         <v>45356</v>
       </c>
@@ -6279,7 +6281,7 @@
       <c r="Y67" s="19"/>
       <c r="Z67" s="19"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="27">
         <v>45356</v>
       </c>
@@ -6350,7 +6352,7 @@
       <c r="Y68" s="19"/>
       <c r="Z68" s="19"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="27">
         <v>45356</v>
       </c>
@@ -6421,7 +6423,7 @@
       <c r="Y69" s="19"/>
       <c r="Z69" s="19"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="27">
         <v>45356</v>
       </c>
@@ -6492,7 +6494,7 @@
       <c r="Y70" s="19"/>
       <c r="Z70" s="19"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="27">
         <v>45356</v>
       </c>
@@ -6563,7 +6565,7 @@
       <c r="Y71" s="19"/>
       <c r="Z71" s="19"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="27">
         <v>45356</v>
       </c>
@@ -6634,7 +6636,7 @@
       <c r="Y72" s="19"/>
       <c r="Z72" s="19"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="27">
         <v>45356</v>
       </c>
@@ -6705,7 +6707,7 @@
       <c r="Y73" s="19"/>
       <c r="Z73" s="19"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="27">
         <v>45356</v>
       </c>
@@ -6776,7 +6778,7 @@
       <c r="Y74" s="19"/>
       <c r="Z74" s="19"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="27">
         <v>45356</v>
       </c>
@@ -6847,7 +6849,7 @@
       <c r="Y75" s="19"/>
       <c r="Z75" s="19"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="27">
         <v>45356</v>
       </c>
@@ -6918,7 +6920,7 @@
       <c r="Y76" s="19"/>
       <c r="Z76" s="19"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="27">
         <v>45356</v>
       </c>
@@ -6989,7 +6991,7 @@
       <c r="Y77" s="19"/>
       <c r="Z77" s="19"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="27">
         <v>45356</v>
       </c>
@@ -7060,7 +7062,7 @@
       <c r="Y78" s="19"/>
       <c r="Z78" s="19"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="27">
         <v>45356</v>
       </c>
@@ -7131,7 +7133,7 @@
       <c r="Y79" s="19"/>
       <c r="Z79" s="19"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="27">
         <v>45356</v>
       </c>
@@ -7202,7 +7204,7 @@
       <c r="Y80" s="19"/>
       <c r="Z80" s="19"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="27">
         <v>45356</v>
       </c>
@@ -7273,7 +7275,7 @@
       <c r="Y81" s="19"/>
       <c r="Z81" s="19"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="27">
         <v>45356</v>
       </c>
@@ -7344,7 +7346,7 @@
       <c r="Y82" s="19"/>
       <c r="Z82" s="19"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="27">
         <v>45356</v>
       </c>
@@ -7415,7 +7417,7 @@
       <c r="Y83" s="19"/>
       <c r="Z83" s="19"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="27">
         <v>45356</v>
       </c>
@@ -7486,7 +7488,7 @@
       <c r="Y84" s="19"/>
       <c r="Z84" s="19"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="27">
         <v>45356</v>
       </c>
@@ -7557,7 +7559,7 @@
       <c r="Y85" s="19"/>
       <c r="Z85" s="19"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="27">
         <v>45356</v>
       </c>
@@ -7628,7 +7630,7 @@
       <c r="Y86" s="19"/>
       <c r="Z86" s="19"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="27">
         <v>45356</v>
       </c>
@@ -7699,7 +7701,7 @@
       <c r="Y87" s="19"/>
       <c r="Z87" s="19"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="27">
         <v>45356</v>
       </c>
@@ -7770,7 +7772,7 @@
       <c r="Y88" s="19"/>
       <c r="Z88" s="19"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="27">
         <v>45356</v>
       </c>
@@ -7841,7 +7843,7 @@
       <c r="Y89" s="19"/>
       <c r="Z89" s="19"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="27">
         <v>45356</v>
       </c>
@@ -7912,7 +7914,7 @@
       <c r="Y90" s="19"/>
       <c r="Z90" s="19"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="27">
         <v>45356</v>
       </c>
@@ -7983,7 +7985,7 @@
       <c r="Y91" s="19"/>
       <c r="Z91" s="19"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="27">
         <v>45356</v>
       </c>
@@ -8054,7 +8056,7 @@
       <c r="Y92" s="19"/>
       <c r="Z92" s="19"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="27">
         <v>45356</v>
       </c>
@@ -8125,7 +8127,7 @@
       <c r="Y93" s="19"/>
       <c r="Z93" s="19"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="27">
         <v>45356</v>
       </c>
@@ -8196,7 +8198,7 @@
       <c r="Y94" s="19"/>
       <c r="Z94" s="19"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="27">
         <v>45356</v>
       </c>
@@ -8267,7 +8269,7 @@
       <c r="Y95" s="19"/>
       <c r="Z95" s="19"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="27">
         <v>45356</v>
       </c>
@@ -8338,7 +8340,7 @@
       <c r="Y96" s="19"/>
       <c r="Z96" s="19"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="27">
         <v>45356</v>
       </c>
@@ -8409,7 +8411,7 @@
       <c r="Y97" s="19"/>
       <c r="Z97" s="19"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="27">
         <v>45356</v>
       </c>
@@ -8480,7 +8482,7 @@
       <c r="Y98" s="19"/>
       <c r="Z98" s="19"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="27">
         <v>45356</v>
       </c>
@@ -8551,7 +8553,7 @@
       <c r="Y99" s="19"/>
       <c r="Z99" s="19"/>
     </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="27">
         <v>45356</v>
       </c>
@@ -8622,7 +8624,7 @@
       <c r="Y100" s="19"/>
       <c r="Z100" s="19"/>
     </row>
-    <row r="101" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="27">
         <v>45356</v>
       </c>
@@ -8693,7 +8695,7 @@
       <c r="Y101" s="19"/>
       <c r="Z101" s="19"/>
     </row>
-    <row r="102" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="27">
         <v>45356</v>
       </c>
@@ -8764,7 +8766,7 @@
       <c r="Y102" s="19"/>
       <c r="Z102" s="19"/>
     </row>
-    <row r="103" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="27">
         <v>45356</v>
       </c>
@@ -8835,7 +8837,7 @@
       <c r="Y103" s="19"/>
       <c r="Z103" s="19"/>
     </row>
-    <row r="104" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="27">
         <v>45356</v>
       </c>
@@ -8906,7 +8908,7 @@
       <c r="Y104" s="19"/>
       <c r="Z104" s="19"/>
     </row>
-    <row r="105" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="27">
         <v>45356</v>
       </c>
@@ -8977,7 +8979,7 @@
       <c r="Y105" s="19"/>
       <c r="Z105" s="19"/>
     </row>
-    <row r="106" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="27">
         <v>45356</v>
       </c>
@@ -9048,7 +9050,7 @@
       <c r="Y106" s="19"/>
       <c r="Z106" s="19"/>
     </row>
-    <row r="107" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="28">
         <v>45356</v>
       </c>
@@ -9119,10 +9121,10 @@
       <c r="Y107" s="15"/>
       <c r="Z107" s="15"/>
     </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D123" s="1"/>
     </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="4:4" x14ac:dyDescent="0.55000000000000004">
       <c r="D124" s="1"/>
     </row>
   </sheetData>
@@ -9139,14 +9141,14 @@
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="42.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="42.26171875" customWidth="1"/>
+    <col min="2" max="2" width="19.578125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>153</v>
       </c>
@@ -9160,7 +9162,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>157</v>
       </c>
@@ -9174,7 +9176,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>160</v>
       </c>
@@ -9188,7 +9190,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>162</v>
       </c>
@@ -9202,7 +9204,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>164</v>
       </c>
@@ -9216,7 +9218,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>165</v>
       </c>
@@ -9230,7 +9232,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
         <v>167</v>
       </c>
@@ -9244,7 +9246,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
         <v>169</v>
       </c>
@@ -9258,7 +9260,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>171</v>
       </c>

</xml_diff>

<commit_message>
updated data by heike
</commit_message>
<xml_diff>
--- a/FSP_Exchange/data/Overview_Stat_Analyses.xlsx
+++ b/FSP_Exchange/data/Overview_Stat_Analyses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefa\OneDrive\Dokumente\Career\Freelance\_Kunden\BRAHMS\2024 - FSP\fsp_validation\FSP_Exchange\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thermofisher-my.sharepoint.com/personal/heike_goehler_thermofisher_com/Documents/FSP_Exchange/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECA2313-BEC1-4E64-9016-914F5FE7E831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="441" documentId="8_{B71B119A-91B9-41B4-A31F-26ADBC8182F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FC3664A-D6A9-4D68-A67B-8EC85620F36D}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{DB58F8A3-982D-4375-901B-E1B15CF4D99D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{DB58F8A3-982D-4375-901B-E1B15CF4D99D}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1827" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1847" uniqueCount="246">
   <si>
     <t>Analysis</t>
   </si>
@@ -423,9 +423,6 @@
     <t>AFP, hCGß, uE3, InhibinA</t>
   </si>
   <si>
-    <t>4_FMF_UK_A1</t>
-  </si>
-  <si>
     <t>12T_Triso_ T21</t>
   </si>
   <si>
@@ -769,6 +766,15 @@
   </si>
   <si>
     <t>7_FMF_UK_A4b</t>
+  </si>
+  <si>
+    <t>4_FMF_UK_A1a</t>
+  </si>
+  <si>
+    <t>4_FMF_UK_A1b</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -964,7 +970,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1029,9 +1035,19 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1096,9 +1112,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1136,7 +1152,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1242,7 +1258,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1384,7 +1400,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1392,45 +1408,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D59CA7-78DE-483F-8DC5-D261426A3AA3}">
-  <dimension ref="A1:AL124"/>
+  <dimension ref="A1:AL125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="T10" sqref="T10"/>
+      <selection pane="bottomRight" activeCell="P54" sqref="P54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.68359375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="16.26171875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="20.578125" customWidth="1"/>
-    <col min="4" max="4" width="5.578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.41796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.41796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.68359375" customWidth="1"/>
-    <col min="8" max="8" width="37.26171875" customWidth="1"/>
-    <col min="9" max="9" width="10.83984375" customWidth="1"/>
-    <col min="10" max="10" width="12.15625" customWidth="1"/>
-    <col min="11" max="11" width="15.68359375" customWidth="1"/>
-    <col min="12" max="12" width="33.41796875" customWidth="1"/>
-    <col min="13" max="13" width="28.41796875" customWidth="1"/>
-    <col min="14" max="14" width="23.15625" customWidth="1"/>
-    <col min="15" max="15" width="13.41796875" customWidth="1"/>
-    <col min="16" max="16" width="12.68359375" customWidth="1"/>
-    <col min="17" max="17" width="21.41796875" customWidth="1"/>
-    <col min="18" max="18" width="10.41796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.41796875" customWidth="1"/>
-    <col min="20" max="20" width="22.68359375" customWidth="1"/>
-    <col min="21" max="21" width="10.41796875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.83984375" customWidth="1"/>
-    <col min="23" max="23" width="31.68359375" customWidth="1"/>
-    <col min="24" max="24" width="21.83984375" customWidth="1"/>
-    <col min="25" max="26" width="21.26171875" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" customWidth="1"/>
+    <col min="8" max="8" width="37.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="33.42578125" customWidth="1"/>
+    <col min="13" max="13" width="28.42578125" customWidth="1"/>
+    <col min="14" max="14" width="23.140625" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" customWidth="1"/>
+    <col min="17" max="17" width="21.42578125" customWidth="1"/>
+    <col min="18" max="18" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" customWidth="1"/>
+    <col min="20" max="20" width="22.7109375" customWidth="1"/>
+    <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.85546875" customWidth="1"/>
+    <col min="23" max="23" width="31.7109375" customWidth="1"/>
+    <col min="24" max="24" width="21.85546875" customWidth="1"/>
+    <col min="25" max="26" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
@@ -1464,7 +1480,7 @@
       <c r="Y1" s="35"/>
       <c r="Z1" s="35"/>
     </row>
-    <row r="2" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>3</v>
       </c>
@@ -1535,16 +1551,16 @@
         <v>25</v>
       </c>
       <c r="X2" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y2" s="25" t="s">
         <v>232</v>
       </c>
-      <c r="Y2" s="25" t="s">
+      <c r="Z2" s="25" t="s">
         <v>233</v>
       </c>
-      <c r="Z2" s="25" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="27">
         <v>45334</v>
       </c>
@@ -1562,7 +1578,7 @@
         <v>27</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H3" s="2" t="str">
         <f>F3&amp;"_"&amp;C3</f>
@@ -1623,7 +1639,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="27">
         <v>45334</v>
       </c>
@@ -1641,7 +1657,7 @@
         <v>27</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H4" s="2" t="str">
         <f t="shared" ref="H4:H19" si="0">F4&amp;"_"&amp;C4</f>
@@ -1702,7 +1718,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
         <v>45334</v>
       </c>
@@ -1720,7 +1736,7 @@
         <v>27</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1781,7 +1797,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
         <v>45334</v>
       </c>
@@ -1850,17 +1866,17 @@
       <c r="W6" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="X6" s="19" t="s">
-        <v>235</v>
+      <c r="X6" s="38">
+        <v>109</v>
       </c>
       <c r="Y6" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Z6" s="19">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="27">
         <v>45334</v>
       </c>
@@ -1929,17 +1945,17 @@
       <c r="W7" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="X7" s="19" t="s">
-        <v>235</v>
+      <c r="X7" s="38">
+        <v>109</v>
       </c>
       <c r="Y7" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Z7" s="19">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="28">
         <v>45334</v>
       </c>
@@ -2008,17 +2024,17 @@
       <c r="W8" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="X8" s="15" t="s">
-        <v>235</v>
+      <c r="X8" s="39">
+        <v>109</v>
       </c>
       <c r="Y8" s="15" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Z8" s="15">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
         <v>45334</v>
       </c>
@@ -2026,14 +2042,14 @@
         <v>45337</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D9" s="24">
         <v>1</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>50</v>
@@ -2097,7 +2113,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
         <v>45334</v>
       </c>
@@ -2105,14 +2121,14 @@
         <v>45337</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D10" s="24">
         <v>1</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>50</v>
@@ -2143,7 +2159,7 @@
         <v>32</v>
       </c>
       <c r="P10" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="Q10" s="20" t="s">
         <v>31</v>
@@ -2176,7 +2192,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="27">
         <v>45334</v>
       </c>
@@ -2191,7 +2207,7 @@
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>56</v>
@@ -2222,7 +2238,7 @@
         <v>32</v>
       </c>
       <c r="P11" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="Q11" s="20" t="s">
         <v>31</v>
@@ -2255,7 +2271,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="28">
         <v>45334</v>
       </c>
@@ -2270,7 +2286,7 @@
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>59</v>
@@ -2334,7 +2350,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="27">
         <v>45334</v>
       </c>
@@ -2349,7 +2365,7 @@
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>62</v>
@@ -2413,7 +2429,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="27">
         <v>45334</v>
       </c>
@@ -2421,14 +2437,14 @@
         <v>45337</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D14" s="24">
         <v>2</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>67</v>
@@ -2492,7 +2508,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="27">
         <v>45334</v>
       </c>
@@ -2500,14 +2516,14 @@
         <v>45337</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D15" s="24">
         <v>2</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>67</v>
@@ -2538,7 +2554,7 @@
         <v>65</v>
       </c>
       <c r="P15" s="37" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Q15" s="20" t="s">
         <v>31</v>
@@ -2552,9 +2568,15 @@
       <c r="T15" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="U15" s="31"/>
-      <c r="V15" s="20"/>
-      <c r="W15" s="20"/>
+      <c r="U15" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="V15" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="W15" s="20" t="s">
+        <v>31</v>
+      </c>
       <c r="X15" s="19">
         <v>47</v>
       </c>
@@ -2565,7 +2587,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="27">
         <v>45334</v>
       </c>
@@ -2580,7 +2602,7 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>69</v>
@@ -2644,7 +2666,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="27">
         <v>45334</v>
       </c>
@@ -2652,14 +2674,14 @@
         <v>45337</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D17" s="24">
         <v>12</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>70</v>
@@ -2723,7 +2745,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="27">
         <v>45334</v>
       </c>
@@ -2731,14 +2753,14 @@
         <v>45337</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D18" s="24">
         <v>12</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>70</v>
@@ -2769,7 +2791,7 @@
         <v>65</v>
       </c>
       <c r="P18" s="37" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Q18" s="20" t="s">
         <v>31</v>
@@ -2783,9 +2805,15 @@
       <c r="T18" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="U18" s="31"/>
-      <c r="V18" s="20"/>
-      <c r="W18" s="20"/>
+      <c r="U18" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="V18" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="W18" s="20" t="s">
+        <v>31</v>
+      </c>
       <c r="X18" s="19">
         <v>47</v>
       </c>
@@ -2796,7 +2824,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="28">
         <v>45334</v>
       </c>
@@ -2811,7 +2839,7 @@
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>72</v>
@@ -2875,7 +2903,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="27">
         <v>45343</v>
       </c>
@@ -2946,7 +2974,7 @@
       <c r="Y20" s="19"/>
       <c r="Z20" s="19"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="28">
         <v>45343</v>
       </c>
@@ -3017,7 +3045,7 @@
       <c r="Y21" s="15"/>
       <c r="Z21" s="15"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="27">
         <v>45343</v>
       </c>
@@ -3036,7 +3064,7 @@
       </c>
       <c r="G22" s="8"/>
       <c r="H22" s="2" t="str">
-        <f t="shared" ref="H22:H106" si="3">F22&amp;"_"&amp;C22</f>
+        <f t="shared" ref="H22:H107" si="3">F22&amp;"_"&amp;C22</f>
         <v>1T_Triso_2_FMF_UK_A1</v>
       </c>
       <c r="I22" s="11">
@@ -3088,7 +3116,7 @@
       <c r="Y22" s="11"/>
       <c r="Z22" s="11"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="27">
         <v>45343</v>
       </c>
@@ -3159,7 +3187,7 @@
       <c r="Y23" s="19"/>
       <c r="Z23" s="19"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="27">
         <v>45343</v>
       </c>
@@ -3230,7 +3258,7 @@
       <c r="Y24" s="19"/>
       <c r="Z24" s="19"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="27">
         <v>45343</v>
       </c>
@@ -3301,7 +3329,7 @@
       <c r="Y25" s="19"/>
       <c r="Z25" s="19"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="27">
         <v>45343</v>
       </c>
@@ -3372,7 +3400,7 @@
       <c r="Y26" s="19"/>
       <c r="Z26" s="19"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="27">
         <v>45343</v>
       </c>
@@ -3441,7 +3469,7 @@
       <c r="Y27" s="19"/>
       <c r="Z27" s="19"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="27">
         <v>45343</v>
       </c>
@@ -3510,7 +3538,7 @@
       <c r="Y28" s="19"/>
       <c r="Z28" s="19"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="27">
         <v>45343</v>
       </c>
@@ -3581,7 +3609,7 @@
       <c r="Y29" s="19"/>
       <c r="Z29" s="19"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="27">
         <v>45343</v>
       </c>
@@ -3652,7 +3680,7 @@
       <c r="Y30" s="19"/>
       <c r="Z30" s="19"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="27">
         <v>45343</v>
       </c>
@@ -3660,14 +3688,14 @@
         <v>45348</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D31" s="19">
         <v>2</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G31" s="5"/>
       <c r="H31" s="2" t="str">
@@ -3723,7 +3751,7 @@
       <c r="Y31" s="19"/>
       <c r="Z31" s="19"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="27">
         <v>45343</v>
       </c>
@@ -3731,14 +3759,14 @@
         <v>45348</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D32" s="19">
         <v>2</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G32" s="5"/>
       <c r="H32" s="2" t="str">
@@ -3794,7 +3822,7 @@
       <c r="Y32" s="19"/>
       <c r="Z32" s="19"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="27">
         <v>45343</v>
       </c>
@@ -3802,14 +3830,14 @@
         <v>45348</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D33" s="19">
         <v>10</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G33" s="5"/>
       <c r="H33" s="2" t="str">
@@ -3865,7 +3893,7 @@
       <c r="Y33" s="19"/>
       <c r="Z33" s="19"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="28">
         <v>45343</v>
       </c>
@@ -3873,14 +3901,14 @@
         <v>45348</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D34" s="19">
         <v>10</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="6" t="str">
@@ -3936,7 +3964,7 @@
       <c r="Y34" s="19"/>
       <c r="Z34" s="19"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="27">
         <v>45348</v>
       </c>
@@ -4007,7 +4035,7 @@
       <c r="Y35" s="11"/>
       <c r="Z35" s="11"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="27">
         <v>45348</v>
       </c>
@@ -4078,7 +4106,7 @@
       <c r="Y36" s="19"/>
       <c r="Z36" s="19"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="27">
         <v>45348</v>
       </c>
@@ -4149,7 +4177,7 @@
       <c r="Y37" s="19"/>
       <c r="Z37" s="19"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="27">
         <v>45348</v>
       </c>
@@ -4220,7 +4248,7 @@
       <c r="Y38" s="19"/>
       <c r="Z38" s="19"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="27">
         <v>45348</v>
       </c>
@@ -4291,7 +4319,7 @@
       <c r="Y39" s="19"/>
       <c r="Z39" s="19"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="27">
         <v>45348</v>
       </c>
@@ -4362,7 +4390,7 @@
       <c r="Y40" s="19"/>
       <c r="Z40" s="19"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="27">
         <v>45348</v>
       </c>
@@ -4370,14 +4398,14 @@
         <v>45351</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D41" s="19">
         <v>8</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G41" s="5"/>
       <c r="H41" s="2" t="str">
@@ -4433,7 +4461,7 @@
       <c r="Y41" s="19"/>
       <c r="Z41" s="19"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="27">
         <v>45348</v>
       </c>
@@ -4441,14 +4469,14 @@
         <v>45351</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D42" s="19">
         <v>8</v>
       </c>
       <c r="E42" s="5"/>
       <c r="F42" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G42" s="5"/>
       <c r="H42" s="2" t="str">
@@ -4504,7 +4532,7 @@
       <c r="Y42" s="19"/>
       <c r="Z42" s="19"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="27">
         <v>45348</v>
       </c>
@@ -4512,14 +4540,14 @@
         <v>45351</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D43" s="19">
         <v>9</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G43" s="5"/>
       <c r="H43" s="2" t="str">
@@ -4575,7 +4603,7 @@
       <c r="Y43" s="19"/>
       <c r="Z43" s="19"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="27">
         <v>45348</v>
       </c>
@@ -4583,14 +4611,14 @@
         <v>45351</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D44" s="19">
         <v>9</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G44" s="5"/>
       <c r="H44" s="2" t="str">
@@ -4646,7 +4674,7 @@
       <c r="Y44" s="19"/>
       <c r="Z44" s="19"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="27">
         <v>45348</v>
       </c>
@@ -4654,14 +4682,14 @@
         <v>45351</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D45" s="19">
         <v>11</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G45" s="5"/>
       <c r="H45" s="2" t="str">
@@ -4717,7 +4745,7 @@
       <c r="Y45" s="19"/>
       <c r="Z45" s="19"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="27">
         <v>45348</v>
       </c>
@@ -4725,14 +4753,14 @@
         <v>45351</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D46" s="19">
         <v>11</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G46" s="5"/>
       <c r="H46" s="2" t="str">
@@ -4788,7 +4816,7 @@
       <c r="Y46" s="19"/>
       <c r="Z46" s="19"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="27">
         <v>45348</v>
       </c>
@@ -4796,14 +4824,14 @@
         <v>45351</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D47" s="19">
         <v>12</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G47" s="5"/>
       <c r="H47" s="2" t="str">
@@ -4859,7 +4887,7 @@
       <c r="Y47" s="19"/>
       <c r="Z47" s="19"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="27">
         <v>45348</v>
       </c>
@@ -4867,14 +4895,14 @@
         <v>45351</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D48" s="19">
         <v>12</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G48" s="5"/>
       <c r="H48" s="2" t="str">
@@ -4930,7 +4958,7 @@
       <c r="Y48" s="19"/>
       <c r="Z48" s="19"/>
     </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A49" s="27">
         <v>45348</v>
       </c>
@@ -4938,14 +4966,14 @@
         <v>45351</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D49" s="19">
         <v>4</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G49" s="5"/>
       <c r="H49" s="2" t="str">
@@ -5001,7 +5029,7 @@
       <c r="Y49" s="19"/>
       <c r="Z49" s="19"/>
     </row>
-    <row r="50" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A50" s="27">
         <v>45348</v>
       </c>
@@ -5009,14 +5037,14 @@
         <v>45351</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D50" s="19">
         <v>4</v>
       </c>
       <c r="E50" s="5"/>
       <c r="F50" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G50" s="5"/>
       <c r="H50" s="2" t="str">
@@ -5072,7 +5100,7 @@
       <c r="Y50" s="19"/>
       <c r="Z50" s="19"/>
     </row>
-    <row r="51" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A51" s="27">
         <v>45348</v>
       </c>
@@ -5080,14 +5108,14 @@
         <v>45351</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D51" s="19">
         <v>10</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G51" s="5"/>
       <c r="H51" s="2" t="str">
@@ -5144,7 +5172,7 @@
       <c r="Z51" s="19"/>
       <c r="AL51" s="33"/>
     </row>
-    <row r="52" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A52" s="28">
         <v>45348</v>
       </c>
@@ -5152,14 +5180,14 @@
         <v>45351</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D52" s="19">
         <v>10</v>
       </c>
       <c r="E52" s="5"/>
       <c r="F52" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G52" s="5"/>
       <c r="H52" s="6" t="str">
@@ -5216,7 +5244,7 @@
       <c r="Z52" s="19"/>
       <c r="AL52" s="33"/>
     </row>
-    <row r="53" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A53" s="27">
         <v>45356</v>
       </c>
@@ -5224,31 +5252,31 @@
         <v>45359</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>128</v>
+        <v>243</v>
       </c>
       <c r="D53" s="11">
         <v>1</v>
       </c>
       <c r="E53" s="8"/>
       <c r="F53" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G53" s="8"/>
       <c r="H53" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>12T_Triso_ T21_4_FMF_UK_A1</v>
+        <v>12T_Triso_ T21_4_FMF_UK_A1a</v>
       </c>
       <c r="I53" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J53" s="8" t="s">
         <v>28</v>
       </c>
       <c r="K53" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="L53" s="8" t="s">
         <v>131</v>
-      </c>
-      <c r="L53" s="8" t="s">
-        <v>132</v>
       </c>
       <c r="M53" s="8" t="s">
         <v>111</v>
@@ -5287,54 +5315,54 @@
       <c r="Y53" s="11"/>
       <c r="Z53" s="11"/>
     </row>
-    <row r="54" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A54" s="27">
         <v>45356</v>
       </c>
       <c r="B54" s="27">
         <v>45359</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D54" s="19">
-        <v>2</v>
-      </c>
-      <c r="E54" s="5"/>
-      <c r="F54" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G54" s="5"/>
+      <c r="C54" s="40" t="s">
+        <v>244</v>
+      </c>
+      <c r="D54" s="41">
+        <v>1</v>
+      </c>
+      <c r="E54" s="40"/>
+      <c r="F54" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="G54" s="40"/>
       <c r="H54" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_single_sim_4_FMF_UK_A2</v>
+        <v>12T_Triso_ T21_4_FMF_UK_A1b</v>
       </c>
       <c r="I54" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K54" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="J54" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="K54" s="18" t="s">
+      <c r="L54" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L54" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="M54" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="N54" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="O54" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="N54" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="O54" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="P54" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q54" s="20" t="s">
-        <v>31</v>
+      <c r="P54" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q54" s="2" t="s">
+        <v>245</v>
       </c>
       <c r="R54" s="31" t="s">
         <v>88</v>
@@ -5354,11 +5382,11 @@
       <c r="W54" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="X54" s="19"/>
-      <c r="Y54" s="19"/>
-      <c r="Z54" s="19"/>
-    </row>
-    <row r="55" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+      <c r="X54" s="41"/>
+      <c r="Y54" s="41"/>
+      <c r="Z54" s="41"/>
+    </row>
+    <row r="55" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A55" s="27">
         <v>45356</v>
       </c>
@@ -5366,10 +5394,10 @@
         <v>45359</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D55" s="19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="2" t="s">
@@ -5378,27 +5406,27 @@
       <c r="G55" s="5"/>
       <c r="H55" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_single_sim_4_FMF_UK_A3</v>
+        <v>Triso_single_sim_4_FMF_UK_A2</v>
       </c>
       <c r="I55" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J55" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K55" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="L55" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L55" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="M55" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="N55" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="O55" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="N55" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="O55" s="20" t="s">
         <v>77</v>
       </c>
       <c r="P55" s="20" t="s">
@@ -5429,7 +5457,7 @@
       <c r="Y55" s="19"/>
       <c r="Z55" s="19"/>
     </row>
-    <row r="56" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A56" s="27">
         <v>45356</v>
       </c>
@@ -5437,10 +5465,10 @@
         <v>45359</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D56" s="19">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="E56" s="5"/>
       <c r="F56" s="2" t="s">
@@ -5449,27 +5477,27 @@
       <c r="G56" s="5"/>
       <c r="H56" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_single_sim_4_FMF_UK_A4</v>
+        <v>Triso_single_sim_4_FMF_UK_A3</v>
       </c>
       <c r="I56" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K56" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="L56" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L56" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="M56" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="N56" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="O56" s="18" t="s">
+      <c r="O56" s="31" t="s">
         <v>77</v>
       </c>
       <c r="P56" s="20" t="s">
@@ -5500,7 +5528,7 @@
       <c r="Y56" s="19"/>
       <c r="Z56" s="19"/>
     </row>
-    <row r="57" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A57" s="27">
         <v>45356</v>
       </c>
@@ -5508,10 +5536,10 @@
         <v>45359</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D57" s="19">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E57" s="5"/>
       <c r="F57" s="2" t="s">
@@ -5520,27 +5548,27 @@
       <c r="G57" s="5"/>
       <c r="H57" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_single_sim_4_FMF_UK_A5</v>
+        <v>Triso_single_sim_4_FMF_UK_A4</v>
       </c>
       <c r="I57" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J57" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K57" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="L57" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L57" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="M57" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="N57" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="O57" s="31" t="s">
+      <c r="O57" s="18" t="s">
         <v>77</v>
       </c>
       <c r="P57" s="20" t="s">
@@ -5571,7 +5599,7 @@
       <c r="Y57" s="19"/>
       <c r="Z57" s="19"/>
     </row>
-    <row r="58" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A58" s="27">
         <v>45356</v>
       </c>
@@ -5579,10 +5607,10 @@
         <v>45359</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D58" s="19">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="E58" s="5"/>
       <c r="F58" s="2" t="s">
@@ -5591,22 +5619,22 @@
       <c r="G58" s="5"/>
       <c r="H58" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_single_sim_4_FMF_UK_A6</v>
+        <v>Triso_single_sim_4_FMF_UK_A5</v>
       </c>
       <c r="I58" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K58" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="L58" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L58" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="M58" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="N58" s="20" t="s">
         <v>31</v>
@@ -5642,7 +5670,7 @@
       <c r="Y58" s="19"/>
       <c r="Z58" s="19"/>
     </row>
-    <row r="59" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A59" s="27">
         <v>45356</v>
       </c>
@@ -5650,10 +5678,10 @@
         <v>45359</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D59" s="19">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E59" s="5"/>
       <c r="F59" s="2" t="s">
@@ -5662,27 +5690,27 @@
       <c r="G59" s="5"/>
       <c r="H59" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_single_sim_4_FMF_UK_A7</v>
+        <v>Triso_single_sim_4_FMF_UK_A6</v>
       </c>
       <c r="I59" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K59" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="L59" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L59" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="M59" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="N59" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="O59" s="18" t="s">
+      <c r="O59" s="31" t="s">
         <v>77</v>
       </c>
       <c r="P59" s="20" t="s">
@@ -5713,7 +5741,7 @@
       <c r="Y59" s="19"/>
       <c r="Z59" s="19"/>
     </row>
-    <row r="60" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A60" s="27">
         <v>45356</v>
       </c>
@@ -5721,10 +5749,10 @@
         <v>45359</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D60" s="19">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E60" s="5"/>
       <c r="F60" s="2" t="s">
@@ -5733,27 +5761,27 @@
       <c r="G60" s="5"/>
       <c r="H60" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_single_sim_4_FMF_UK_A8</v>
+        <v>Triso_single_sim_4_FMF_UK_A7</v>
       </c>
       <c r="I60" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K60" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="L60" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L60" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="M60" s="2" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="N60" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="O60" s="31" t="s">
+      <c r="O60" s="18" t="s">
         <v>77</v>
       </c>
       <c r="P60" s="20" t="s">
@@ -5784,7 +5812,7 @@
       <c r="Y60" s="19"/>
       <c r="Z60" s="19"/>
     </row>
-    <row r="61" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A61" s="27">
         <v>45356</v>
       </c>
@@ -5792,10 +5820,10 @@
         <v>45359</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D61" s="19">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E61" s="5"/>
       <c r="F61" s="2" t="s">
@@ -5804,22 +5832,22 @@
       <c r="G61" s="5"/>
       <c r="H61" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_single_sim_4_FMF_UK_A9</v>
+        <v>Triso_single_sim_4_FMF_UK_A8</v>
       </c>
       <c r="I61" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J61" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K61" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M61" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="N61" s="20" t="s">
         <v>31</v>
@@ -5855,7 +5883,7 @@
       <c r="Y61" s="19"/>
       <c r="Z61" s="19"/>
     </row>
-    <row r="62" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A62" s="27">
         <v>45356</v>
       </c>
@@ -5863,10 +5891,10 @@
         <v>45359</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D62" s="19">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E62" s="5"/>
       <c r="F62" s="2" t="s">
@@ -5875,27 +5903,27 @@
       <c r="G62" s="5"/>
       <c r="H62" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_single_sim_4_FMF_UK_A10</v>
+        <v>Triso_single_sim_4_FMF_UK_A9</v>
       </c>
       <c r="I62" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J62" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K62" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M62" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="N62" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="O62" s="18" t="s">
+      <c r="O62" s="31" t="s">
         <v>77</v>
       </c>
       <c r="P62" s="20" t="s">
@@ -5926,7 +5954,7 @@
       <c r="Y62" s="19"/>
       <c r="Z62" s="19"/>
     </row>
-    <row r="63" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A63" s="27">
         <v>45356</v>
       </c>
@@ -5934,10 +5962,10 @@
         <v>45359</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D63" s="19">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E63" s="5"/>
       <c r="F63" s="2" t="s">
@@ -5946,27 +5974,27 @@
       <c r="G63" s="5"/>
       <c r="H63" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_single_sim_4_FMF_UK_A11</v>
+        <v>Triso_single_sim_4_FMF_UK_A10</v>
       </c>
       <c r="I63" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J63" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K63" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M63" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="N63" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="O63" s="31" t="s">
+      <c r="O63" s="18" t="s">
         <v>77</v>
       </c>
       <c r="P63" s="20" t="s">
@@ -5997,7 +6025,7 @@
       <c r="Y63" s="19"/>
       <c r="Z63" s="19"/>
     </row>
-    <row r="64" spans="1:38" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A64" s="27">
         <v>45356</v>
       </c>
@@ -6005,10 +6033,10 @@
         <v>45359</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D64" s="19">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="E64" s="5"/>
       <c r="F64" s="2" t="s">
@@ -6017,22 +6045,22 @@
       <c r="G64" s="5"/>
       <c r="H64" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_single_sim_4_FMF_UK_A12</v>
+        <v>Triso_single_sim_4_FMF_UK_A11</v>
       </c>
       <c r="I64" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J64" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K64" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M64" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="N64" s="20" t="s">
         <v>31</v>
@@ -6068,7 +6096,7 @@
       <c r="Y64" s="19"/>
       <c r="Z64" s="19"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="27">
         <v>45356</v>
       </c>
@@ -6076,10 +6104,10 @@
         <v>45359</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D65" s="19">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E65" s="5"/>
       <c r="F65" s="2" t="s">
@@ -6088,27 +6116,27 @@
       <c r="G65" s="5"/>
       <c r="H65" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_single_sim_4_FMF_UK_A13</v>
+        <v>Triso_single_sim_4_FMF_UK_A12</v>
       </c>
       <c r="I65" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J65" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K65" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M65" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="N65" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="O65" s="18" t="s">
+      <c r="O65" s="31" t="s">
         <v>77</v>
       </c>
       <c r="P65" s="20" t="s">
@@ -6139,7 +6167,7 @@
       <c r="Y65" s="19"/>
       <c r="Z65" s="19"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="27">
         <v>45356</v>
       </c>
@@ -6147,10 +6175,10 @@
         <v>45359</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D66" s="19">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E66" s="5"/>
       <c r="F66" s="2" t="s">
@@ -6159,27 +6187,27 @@
       <c r="G66" s="5"/>
       <c r="H66" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_single_sim_4_FMF_UK_A14</v>
+        <v>Triso_single_sim_4_FMF_UK_A13</v>
       </c>
       <c r="I66" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J66" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K66" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="M66" s="2" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="N66" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="O66" s="31" t="s">
+      <c r="O66" s="18" t="s">
         <v>77</v>
       </c>
       <c r="P66" s="20" t="s">
@@ -6210,7 +6238,7 @@
       <c r="Y66" s="19"/>
       <c r="Z66" s="19"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="27">
         <v>45356</v>
       </c>
@@ -6218,10 +6246,10 @@
         <v>45359</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D67" s="19">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E67" s="5"/>
       <c r="F67" s="2" t="s">
@@ -6230,22 +6258,22 @@
       <c r="G67" s="5"/>
       <c r="H67" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_single_sim_4_FMF_UK_A15</v>
+        <v>Triso_single_sim_4_FMF_UK_A14</v>
       </c>
       <c r="I67" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J67" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K67" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M67" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="N67" s="20" t="s">
         <v>31</v>
@@ -6281,7 +6309,7 @@
       <c r="Y67" s="19"/>
       <c r="Z67" s="19"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="27">
         <v>45356</v>
       </c>
@@ -6289,10 +6317,10 @@
         <v>45359</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D68" s="19">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E68" s="5"/>
       <c r="F68" s="2" t="s">
@@ -6301,27 +6329,27 @@
       <c r="G68" s="5"/>
       <c r="H68" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_single_sim_4_FMF_UK_A16</v>
+        <v>Triso_single_sim_4_FMF_UK_A15</v>
       </c>
       <c r="I68" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J68" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K68" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M68" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="N68" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="O68" s="18" t="s">
+      <c r="O68" s="31" t="s">
         <v>77</v>
       </c>
       <c r="P68" s="20" t="s">
@@ -6352,7 +6380,7 @@
       <c r="Y68" s="19"/>
       <c r="Z68" s="19"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" s="27">
         <v>45356</v>
       </c>
@@ -6360,10 +6388,10 @@
         <v>45359</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D69" s="19">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E69" s="5"/>
       <c r="F69" s="2" t="s">
@@ -6372,27 +6400,27 @@
       <c r="G69" s="5"/>
       <c r="H69" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_single_sim_4_FMF_UK_A17</v>
+        <v>Triso_single_sim_4_FMF_UK_A16</v>
       </c>
       <c r="I69" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J69" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K69" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M69" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="N69" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="O69" s="31" t="s">
+      <c r="O69" s="18" t="s">
         <v>77</v>
       </c>
       <c r="P69" s="20" t="s">
@@ -6423,7 +6451,7 @@
       <c r="Y69" s="19"/>
       <c r="Z69" s="19"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" s="27">
         <v>45356</v>
       </c>
@@ -6431,10 +6459,10 @@
         <v>45359</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D70" s="19">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="E70" s="5"/>
       <c r="F70" s="2" t="s">
@@ -6443,22 +6471,22 @@
       <c r="G70" s="5"/>
       <c r="H70" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_single_sim_4_FMF_UK_A18</v>
+        <v>Triso_single_sim_4_FMF_UK_A17</v>
       </c>
       <c r="I70" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K70" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="N70" s="20" t="s">
         <v>31</v>
@@ -6494,7 +6522,7 @@
       <c r="Y70" s="19"/>
       <c r="Z70" s="19"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" s="27">
         <v>45356</v>
       </c>
@@ -6502,10 +6530,10 @@
         <v>45359</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D71" s="19">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E71" s="5"/>
       <c r="F71" s="2" t="s">
@@ -6514,27 +6542,27 @@
       <c r="G71" s="5"/>
       <c r="H71" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_single_sim_4_FMF_UK_A19</v>
+        <v>Triso_single_sim_4_FMF_UK_A18</v>
       </c>
       <c r="I71" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J71" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K71" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M71" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="N71" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="O71" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="N71" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="O71" s="31" t="s">
         <v>77</v>
       </c>
       <c r="P71" s="20" t="s">
@@ -6565,7 +6593,7 @@
       <c r="Y71" s="19"/>
       <c r="Z71" s="19"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" s="27">
         <v>45356</v>
       </c>
@@ -6573,39 +6601,39 @@
         <v>45359</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>193</v>
+        <v>151</v>
       </c>
       <c r="D72" s="19">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E72" s="5"/>
       <c r="F72" s="2" t="s">
-        <v>179</v>
+        <v>104</v>
       </c>
       <c r="G72" s="5"/>
       <c r="H72" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_sim_MC_4_FMF_UK_A20_MC</v>
+        <v>Triso_single_sim_4_FMF_UK_A19</v>
       </c>
       <c r="I72" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J72" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K72" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L72" s="2" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="M72" s="2" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="N72" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="O72" s="31" t="s">
+      <c r="O72" s="18" t="s">
         <v>77</v>
       </c>
       <c r="P72" s="20" t="s">
@@ -6636,7 +6664,7 @@
       <c r="Y72" s="19"/>
       <c r="Z72" s="19"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A73" s="27">
         <v>45356</v>
       </c>
@@ -6644,31 +6672,31 @@
         <v>45359</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
       <c r="D73" s="19">
         <v>4</v>
       </c>
       <c r="E73" s="5"/>
       <c r="F73" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G73" s="5"/>
       <c r="H73" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_sim_MC_4_FMF_UK_A20_DC</v>
+        <v>Triso_sim_MC_4_FMF_UK_A20_MC</v>
       </c>
       <c r="I73" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J73" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K73" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="L73" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="L73" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="M73" s="2" t="s">
         <v>111</v>
@@ -6707,7 +6735,7 @@
       <c r="Y73" s="19"/>
       <c r="Z73" s="19"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A74" s="27">
         <v>45356</v>
       </c>
@@ -6715,34 +6743,34 @@
         <v>45359</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="D74" s="19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E74" s="5"/>
       <c r="F74" s="2" t="s">
-        <v>107</v>
+        <v>178</v>
       </c>
       <c r="G74" s="5"/>
       <c r="H74" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A21_MC</v>
+        <v>Triso_sim_MC_4_FMF_UK_A20_DC</v>
       </c>
       <c r="I74" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J74" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K74" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="L74" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L74" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="M74" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="N74" s="21" t="s">
         <v>31</v>
@@ -6778,7 +6806,7 @@
       <c r="Y74" s="19"/>
       <c r="Z74" s="19"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A75" s="27">
         <v>45356</v>
       </c>
@@ -6786,7 +6814,7 @@
         <v>45359</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
       <c r="D75" s="19">
         <v>5</v>
@@ -6798,19 +6826,19 @@
       <c r="G75" s="5"/>
       <c r="H75" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A21_DC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A21_MC</v>
       </c>
       <c r="I75" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J75" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K75" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="L75" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="L75" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="M75" s="2" t="s">
         <v>116</v>
@@ -6849,7 +6877,7 @@
       <c r="Y75" s="19"/>
       <c r="Z75" s="19"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A76" s="27">
         <v>45356</v>
       </c>
@@ -6857,10 +6885,10 @@
         <v>45359</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="D76" s="19">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="E76" s="5"/>
       <c r="F76" s="2" t="s">
@@ -6869,27 +6897,27 @@
       <c r="G76" s="5"/>
       <c r="H76" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A22_MC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A21_DC</v>
       </c>
       <c r="I76" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J76" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K76" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="L76" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L76" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="M76" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="N76" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="O76" s="18" t="s">
+      <c r="O76" s="31" t="s">
         <v>77</v>
       </c>
       <c r="P76" s="20" t="s">
@@ -6920,7 +6948,7 @@
       <c r="Y76" s="19"/>
       <c r="Z76" s="19"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A77" s="27">
         <v>45356</v>
       </c>
@@ -6928,7 +6956,7 @@
         <v>45359</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="D77" s="19">
         <v>28</v>
@@ -6940,19 +6968,19 @@
       <c r="G77" s="5"/>
       <c r="H77" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A22_DC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A22_MC</v>
       </c>
       <c r="I77" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J77" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K77" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="L77" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="L77" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="M77" s="2" t="s">
         <v>118</v>
@@ -6991,7 +7019,7 @@
       <c r="Y77" s="19"/>
       <c r="Z77" s="19"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A78" s="27">
         <v>45356</v>
       </c>
@@ -6999,10 +7027,10 @@
         <v>45359</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="D78" s="19">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E78" s="5"/>
       <c r="F78" s="2" t="s">
@@ -7011,27 +7039,27 @@
       <c r="G78" s="5"/>
       <c r="H78" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A23_MC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A22_DC</v>
       </c>
       <c r="I78" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J78" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K78" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="L78" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L78" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="M78" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="N78" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="O78" s="31" t="s">
+      <c r="O78" s="18" t="s">
         <v>77</v>
       </c>
       <c r="P78" s="20" t="s">
@@ -7062,7 +7090,7 @@
       <c r="Y78" s="19"/>
       <c r="Z78" s="19"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A79" s="27">
         <v>45356</v>
       </c>
@@ -7070,7 +7098,7 @@
         <v>45359</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="D79" s="19">
         <v>29</v>
@@ -7082,19 +7110,19 @@
       <c r="G79" s="5"/>
       <c r="H79" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A23_DC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A23_MC</v>
       </c>
       <c r="I79" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J79" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K79" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="L79" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="L79" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="M79" s="2" t="s">
         <v>120</v>
@@ -7133,7 +7161,7 @@
       <c r="Y79" s="19"/>
       <c r="Z79" s="19"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A80" s="27">
         <v>45356</v>
       </c>
@@ -7141,10 +7169,10 @@
         <v>45359</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="D80" s="19">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E80" s="5"/>
       <c r="F80" s="2" t="s">
@@ -7153,22 +7181,22 @@
       <c r="G80" s="5"/>
       <c r="H80" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A24_MC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A23_DC</v>
       </c>
       <c r="I80" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J80" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K80" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="L80" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L80" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="M80" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="N80" s="21" t="s">
         <v>31</v>
@@ -7204,7 +7232,7 @@
       <c r="Y80" s="19"/>
       <c r="Z80" s="19"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="27">
         <v>45356</v>
       </c>
@@ -7212,7 +7240,7 @@
         <v>45359</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="D81" s="19">
         <v>8</v>
@@ -7224,19 +7252,19 @@
       <c r="G81" s="5"/>
       <c r="H81" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A24_DC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A24_MC</v>
       </c>
       <c r="I81" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J81" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K81" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="L81" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="L81" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="M81" s="2" t="s">
         <v>122</v>
@@ -7275,7 +7303,7 @@
       <c r="Y81" s="19"/>
       <c r="Z81" s="19"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" s="27">
         <v>45356</v>
       </c>
@@ -7283,10 +7311,10 @@
         <v>45359</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="D82" s="19">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E82" s="5"/>
       <c r="F82" s="2" t="s">
@@ -7295,27 +7323,27 @@
       <c r="G82" s="5"/>
       <c r="H82" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A25_MC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A24_DC</v>
       </c>
       <c r="I82" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J82" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K82" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="L82" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L82" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="M82" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="N82" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="O82" s="18" t="s">
+      <c r="O82" s="31" t="s">
         <v>77</v>
       </c>
       <c r="P82" s="20" t="s">
@@ -7346,7 +7374,7 @@
       <c r="Y82" s="19"/>
       <c r="Z82" s="19"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83" s="27">
         <v>45356</v>
       </c>
@@ -7354,7 +7382,7 @@
         <v>45359</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="D83" s="19">
         <v>9</v>
@@ -7366,19 +7394,19 @@
       <c r="G83" s="5"/>
       <c r="H83" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A25_DC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A25_MC</v>
       </c>
       <c r="I83" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J83" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K83" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="L83" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="L83" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="M83" s="2" t="s">
         <v>127</v>
@@ -7417,7 +7445,7 @@
       <c r="Y83" s="19"/>
       <c r="Z83" s="19"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84" s="27">
         <v>45356</v>
       </c>
@@ -7425,10 +7453,10 @@
         <v>45359</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="D84" s="19">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E84" s="5"/>
       <c r="F84" s="2" t="s">
@@ -7437,27 +7465,27 @@
       <c r="G84" s="5"/>
       <c r="H84" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A26_MC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A25_DC</v>
       </c>
       <c r="I84" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J84" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K84" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="L84" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L84" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="M84" s="2" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="N84" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="O84" s="31" t="s">
+      <c r="O84" s="18" t="s">
         <v>77</v>
       </c>
       <c r="P84" s="20" t="s">
@@ -7488,7 +7516,7 @@
       <c r="Y84" s="19"/>
       <c r="Z84" s="19"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85" s="27">
         <v>45356</v>
       </c>
@@ -7496,7 +7524,7 @@
         <v>45359</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="D85" s="19">
         <v>20</v>
@@ -7508,19 +7536,19 @@
       <c r="G85" s="5"/>
       <c r="H85" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A26_DC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A26_MC</v>
       </c>
       <c r="I85" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J85" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K85" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L85" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M85" s="2" t="s">
         <v>111</v>
@@ -7559,7 +7587,7 @@
       <c r="Y85" s="19"/>
       <c r="Z85" s="19"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A86" s="27">
         <v>45356</v>
       </c>
@@ -7567,10 +7595,10 @@
         <v>45359</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>200</v>
+        <v>216</v>
       </c>
       <c r="D86" s="19">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E86" s="5"/>
       <c r="F86" s="2" t="s">
@@ -7579,27 +7607,27 @@
       <c r="G86" s="5"/>
       <c r="H86" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A27_MC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A26_DC</v>
       </c>
       <c r="I86" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J86" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K86" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L86" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M86" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="N86" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="O86" s="18" t="s">
+      <c r="O86" s="31" t="s">
         <v>77</v>
       </c>
       <c r="P86" s="20" t="s">
@@ -7630,7 +7658,7 @@
       <c r="Y86" s="19"/>
       <c r="Z86" s="19"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" s="27">
         <v>45356</v>
       </c>
@@ -7638,7 +7666,7 @@
         <v>45359</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="D87" s="19">
         <v>21</v>
@@ -7650,19 +7678,19 @@
       <c r="G87" s="5"/>
       <c r="H87" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A27_DC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A27_MC</v>
       </c>
       <c r="I87" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J87" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K87" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L87" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M87" s="2" t="s">
         <v>116</v>
@@ -7701,7 +7729,7 @@
       <c r="Y87" s="19"/>
       <c r="Z87" s="19"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" s="27">
         <v>45356</v>
       </c>
@@ -7709,10 +7737,10 @@
         <v>45359</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="D88" s="19">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E88" s="5"/>
       <c r="F88" s="2" t="s">
@@ -7721,27 +7749,27 @@
       <c r="G88" s="5"/>
       <c r="H88" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A28_MC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A27_DC</v>
       </c>
       <c r="I88" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J88" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K88" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L88" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M88" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="N88" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="O88" s="31" t="s">
+      <c r="O88" s="18" t="s">
         <v>77</v>
       </c>
       <c r="P88" s="20" t="s">
@@ -7772,7 +7800,7 @@
       <c r="Y88" s="19"/>
       <c r="Z88" s="19"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A89" s="27">
         <v>45356</v>
       </c>
@@ -7780,7 +7808,7 @@
         <v>45359</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="D89" s="19">
         <v>32</v>
@@ -7792,19 +7820,19 @@
       <c r="G89" s="5"/>
       <c r="H89" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A28_DC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A28_MC</v>
       </c>
       <c r="I89" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J89" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K89" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L89" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M89" s="2" t="s">
         <v>118</v>
@@ -7843,7 +7871,7 @@
       <c r="Y89" s="19"/>
       <c r="Z89" s="19"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A90" s="27">
         <v>45356</v>
       </c>
@@ -7851,10 +7879,10 @@
         <v>45359</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>202</v>
+        <v>218</v>
       </c>
       <c r="D90" s="19">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E90" s="5"/>
       <c r="F90" s="2" t="s">
@@ -7863,27 +7891,27 @@
       <c r="G90" s="5"/>
       <c r="H90" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A29_MC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A28_DC</v>
       </c>
       <c r="I90" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J90" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K90" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L90" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M90" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="N90" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="O90" s="18" t="s">
+      <c r="O90" s="31" t="s">
         <v>77</v>
       </c>
       <c r="P90" s="20" t="s">
@@ -7914,7 +7942,7 @@
       <c r="Y90" s="19"/>
       <c r="Z90" s="19"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A91" s="27">
         <v>45356</v>
       </c>
@@ -7922,7 +7950,7 @@
         <v>45359</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="D91" s="19">
         <v>33</v>
@@ -7934,19 +7962,19 @@
       <c r="G91" s="5"/>
       <c r="H91" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A29_DC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A29_MC</v>
       </c>
       <c r="I91" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J91" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K91" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L91" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M91" s="2" t="s">
         <v>120</v>
@@ -7985,7 +8013,7 @@
       <c r="Y91" s="19"/>
       <c r="Z91" s="19"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A92" s="27">
         <v>45356</v>
       </c>
@@ -7993,10 +8021,10 @@
         <v>45359</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="D92" s="19">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="E92" s="5"/>
       <c r="F92" s="2" t="s">
@@ -8005,27 +8033,27 @@
       <c r="G92" s="5"/>
       <c r="H92" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A30_MC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A29_DC</v>
       </c>
       <c r="I92" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J92" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K92" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L92" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M92" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="N92" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="O92" s="31" t="s">
+      <c r="O92" s="18" t="s">
         <v>77</v>
       </c>
       <c r="P92" s="20" t="s">
@@ -8056,7 +8084,7 @@
       <c r="Y92" s="19"/>
       <c r="Z92" s="19"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A93" s="27">
         <v>45356</v>
       </c>
@@ -8064,7 +8092,7 @@
         <v>45359</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
       <c r="D93" s="19">
         <v>12</v>
@@ -8076,19 +8104,19 @@
       <c r="G93" s="5"/>
       <c r="H93" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A30_DC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A30_MC</v>
       </c>
       <c r="I93" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J93" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K93" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L93" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M93" s="2" t="s">
         <v>122</v>
@@ -8127,7 +8155,7 @@
       <c r="Y93" s="19"/>
       <c r="Z93" s="19"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A94" s="27">
         <v>45356</v>
       </c>
@@ -8135,10 +8163,10 @@
         <v>45359</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>204</v>
+        <v>220</v>
       </c>
       <c r="D94" s="19">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E94" s="5"/>
       <c r="F94" s="2" t="s">
@@ -8147,22 +8175,22 @@
       <c r="G94" s="5"/>
       <c r="H94" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A31_MC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A30_DC</v>
       </c>
       <c r="I94" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J94" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K94" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L94" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M94" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="N94" s="21" t="s">
         <v>31</v>
@@ -8198,7 +8226,7 @@
       <c r="Y94" s="19"/>
       <c r="Z94" s="19"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A95" s="27">
         <v>45356</v>
       </c>
@@ -8206,7 +8234,7 @@
         <v>45359</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="D95" s="19">
         <v>13</v>
@@ -8218,19 +8246,19 @@
       <c r="G95" s="5"/>
       <c r="H95" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A31_DC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A31_MC</v>
       </c>
       <c r="I95" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J95" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K95" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L95" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M95" s="2" t="s">
         <v>127</v>
@@ -8269,7 +8297,7 @@
       <c r="Y95" s="19"/>
       <c r="Z95" s="19"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A96" s="27">
         <v>45356</v>
       </c>
@@ -8277,10 +8305,10 @@
         <v>45359</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="D96" s="19">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E96" s="5"/>
       <c r="F96" s="2" t="s">
@@ -8289,27 +8317,27 @@
       <c r="G96" s="5"/>
       <c r="H96" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A32_MC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A31_DC</v>
       </c>
       <c r="I96" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J96" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K96" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L96" s="2" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="M96" s="2" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="N96" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="O96" s="18" t="s">
+      <c r="O96" s="31" t="s">
         <v>77</v>
       </c>
       <c r="P96" s="20" t="s">
@@ -8340,7 +8368,7 @@
       <c r="Y96" s="19"/>
       <c r="Z96" s="19"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A97" s="27">
         <v>45356</v>
       </c>
@@ -8348,7 +8376,7 @@
         <v>45359</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
       <c r="D97" s="19">
         <v>24</v>
@@ -8360,19 +8388,19 @@
       <c r="G97" s="5"/>
       <c r="H97" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A32_DC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A32_MC</v>
       </c>
       <c r="I97" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J97" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K97" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L97" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M97" s="2" t="s">
         <v>111</v>
@@ -8411,7 +8439,7 @@
       <c r="Y97" s="19"/>
       <c r="Z97" s="19"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A98" s="27">
         <v>45356</v>
       </c>
@@ -8419,10 +8447,10 @@
         <v>45359</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="D98" s="19">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E98" s="5"/>
       <c r="F98" s="2" t="s">
@@ -8431,27 +8459,27 @@
       <c r="G98" s="5"/>
       <c r="H98" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A33_MC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A32_DC</v>
       </c>
       <c r="I98" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J98" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K98" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L98" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M98" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="N98" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="O98" s="31" t="s">
+      <c r="O98" s="18" t="s">
         <v>77</v>
       </c>
       <c r="P98" s="20" t="s">
@@ -8482,7 +8510,7 @@
       <c r="Y98" s="19"/>
       <c r="Z98" s="19"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A99" s="27">
         <v>45356</v>
       </c>
@@ -8490,7 +8518,7 @@
         <v>45359</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="D99" s="19">
         <v>25</v>
@@ -8502,19 +8530,19 @@
       <c r="G99" s="5"/>
       <c r="H99" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A33_DC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A33_MC</v>
       </c>
       <c r="I99" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J99" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K99" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L99" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M99" s="2" t="s">
         <v>116</v>
@@ -8553,7 +8581,7 @@
       <c r="Y99" s="19"/>
       <c r="Z99" s="19"/>
     </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A100" s="27">
         <v>45356</v>
       </c>
@@ -8561,10 +8589,10 @@
         <v>45359</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>207</v>
+        <v>223</v>
       </c>
       <c r="D100" s="19">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="E100" s="5"/>
       <c r="F100" s="2" t="s">
@@ -8573,22 +8601,22 @@
       <c r="G100" s="5"/>
       <c r="H100" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A34_MC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A33_DC</v>
       </c>
       <c r="I100" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J100" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K100" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L100" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M100" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="N100" s="21" t="s">
         <v>31</v>
@@ -8624,7 +8652,7 @@
       <c r="Y100" s="19"/>
       <c r="Z100" s="19"/>
     </row>
-    <row r="101" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A101" s="27">
         <v>45356</v>
       </c>
@@ -8632,7 +8660,7 @@
         <v>45359</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="D101" s="19">
         <v>36</v>
@@ -8644,19 +8672,19 @@
       <c r="G101" s="5"/>
       <c r="H101" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A34_DC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A34_MC</v>
       </c>
       <c r="I101" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J101" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K101" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L101" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M101" s="2" t="s">
         <v>118</v>
@@ -8695,7 +8723,7 @@
       <c r="Y101" s="19"/>
       <c r="Z101" s="19"/>
     </row>
-    <row r="102" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A102" s="27">
         <v>45356</v>
       </c>
@@ -8703,10 +8731,10 @@
         <v>45359</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
       <c r="D102" s="19">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E102" s="5"/>
       <c r="F102" s="2" t="s">
@@ -8715,27 +8743,27 @@
       <c r="G102" s="5"/>
       <c r="H102" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A35_MC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A34_DC</v>
       </c>
       <c r="I102" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J102" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K102" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L102" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M102" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="N102" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="O102" s="18" t="s">
+      <c r="O102" s="31" t="s">
         <v>77</v>
       </c>
       <c r="P102" s="20" t="s">
@@ -8766,7 +8794,7 @@
       <c r="Y102" s="19"/>
       <c r="Z102" s="19"/>
     </row>
-    <row r="103" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A103" s="27">
         <v>45356</v>
       </c>
@@ -8774,7 +8802,7 @@
         <v>45359</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
       <c r="D103" s="19">
         <v>37</v>
@@ -8786,19 +8814,19 @@
       <c r="G103" s="5"/>
       <c r="H103" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A35_DC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A35_MC</v>
       </c>
       <c r="I103" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J103" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K103" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L103" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M103" s="2" t="s">
         <v>120</v>
@@ -8837,7 +8865,7 @@
       <c r="Y103" s="19"/>
       <c r="Z103" s="19"/>
     </row>
-    <row r="104" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A104" s="27">
         <v>45356</v>
       </c>
@@ -8845,10 +8873,10 @@
         <v>45359</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>209</v>
+        <v>225</v>
       </c>
       <c r="D104" s="19">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="E104" s="5"/>
       <c r="F104" s="2" t="s">
@@ -8857,27 +8885,27 @@
       <c r="G104" s="5"/>
       <c r="H104" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A36_MC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A35_DC</v>
       </c>
       <c r="I104" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J104" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K104" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L104" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M104" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="N104" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="O104" s="31" t="s">
+      <c r="O104" s="18" t="s">
         <v>77</v>
       </c>
       <c r="P104" s="20" t="s">
@@ -8908,7 +8936,7 @@
       <c r="Y104" s="19"/>
       <c r="Z104" s="19"/>
     </row>
-    <row r="105" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A105" s="27">
         <v>45356</v>
       </c>
@@ -8916,7 +8944,7 @@
         <v>45359</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="D105" s="19">
         <v>16</v>
@@ -8928,19 +8956,19 @@
       <c r="G105" s="5"/>
       <c r="H105" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A36_DC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A36_MC</v>
       </c>
       <c r="I105" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J105" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K105" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L105" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M105" s="2" t="s">
         <v>122</v>
@@ -8979,7 +9007,7 @@
       <c r="Y105" s="19"/>
       <c r="Z105" s="19"/>
     </row>
-    <row r="106" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A106" s="27">
         <v>45356</v>
       </c>
@@ -8987,10 +9015,10 @@
         <v>45359</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
       <c r="D106" s="19">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E106" s="5"/>
       <c r="F106" s="2" t="s">
@@ -8999,27 +9027,27 @@
       <c r="G106" s="5"/>
       <c r="H106" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Triso_twin_sim_4_FMF_UK_A37_MC</v>
+        <v>Triso_twin_sim_4_FMF_UK_A36_DC</v>
       </c>
       <c r="I106" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J106" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="K106" s="2" t="s">
-        <v>131</v>
+      <c r="K106" s="18" t="s">
+        <v>130</v>
       </c>
       <c r="L106" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M106" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="N106" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="O106" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="N106" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="O106" s="31" t="s">
         <v>77</v>
       </c>
       <c r="P106" s="20" t="s">
@@ -9028,7 +9056,7 @@
       <c r="Q106" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="R106" s="20" t="s">
+      <c r="R106" s="31" t="s">
         <v>88</v>
       </c>
       <c r="S106" s="20" t="s">
@@ -9050,82 +9078,153 @@
       <c r="Y106" s="19"/>
       <c r="Z106" s="19"/>
     </row>
-    <row r="107" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A107" s="28">
+    <row r="107" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A107" s="27">
         <v>45356</v>
       </c>
-      <c r="B107" s="28">
+      <c r="B107" s="27">
         <v>45359</v>
       </c>
-      <c r="C107" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="D107" s="15">
+      <c r="C107" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D107" s="19">
         <v>17</v>
       </c>
-      <c r="E107" s="7"/>
-      <c r="F107" s="6" t="s">
+      <c r="E107" s="5"/>
+      <c r="F107" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G107" s="7"/>
-      <c r="H107" s="6" t="str">
-        <f t="shared" ref="H107" si="4">F107&amp;"_"&amp;C107</f>
+      <c r="G107" s="5"/>
+      <c r="H107" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>Triso_twin_sim_4_FMF_UK_A37_MC</v>
+      </c>
+      <c r="I107" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="J107" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K107" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="L107" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="M107" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="N107" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="O107" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="P107" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q107" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="R107" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="S107" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="T107" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="U107" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="V107" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="W107" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="X107" s="19"/>
+      <c r="Y107" s="19"/>
+      <c r="Z107" s="19"/>
+    </row>
+    <row r="108" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A108" s="28">
+        <v>45356</v>
+      </c>
+      <c r="B108" s="28">
+        <v>45359</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="D108" s="15">
+        <v>17</v>
+      </c>
+      <c r="E108" s="7"/>
+      <c r="F108" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G108" s="7"/>
+      <c r="H108" s="6" t="str">
+        <f t="shared" ref="H108" si="4">F108&amp;"_"&amp;C108</f>
         <v>Triso_twin_sim_4_FMF_UK_A37_DC</v>
       </c>
-      <c r="I107" s="15" t="s">
+      <c r="I108" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="J108" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K108" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="J107" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="K107" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="L107" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="M107" s="6" t="s">
+      <c r="L108" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="M108" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="N107" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="O107" s="16" t="s">
+      <c r="N108" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="O108" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="P107" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q107" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="R107" s="16" t="s">
+      <c r="P108" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q108" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="R108" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="S107" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="T107" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="U107" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="V107" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="W107" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="X107" s="15"/>
-      <c r="Y107" s="15"/>
-      <c r="Z107" s="15"/>
-    </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="D123" s="1"/>
-    </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="S108" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="T108" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="U108" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="V108" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="W108" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="X108" s="15"/>
+      <c r="Y108" s="15"/>
+      <c r="Z108" s="15"/>
+    </row>
+    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D124" s="1"/>
+    </row>
+    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D125" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -9141,128 +9240,128 @@
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.26171875" customWidth="1"/>
-    <col min="2" max="2" width="19.578125" customWidth="1"/>
+    <col min="1" max="1" width="42.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" t="s">
         <v>153</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>154</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>155</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>157</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>159</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>160</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="2" t="s">
+      <c r="B4" t="s">
         <v>162</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>163</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="2" t="s">
+      <c r="B6" t="s">
         <v>165</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="2" t="s">
+      <c r="B7" t="s">
         <v>167</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="2" t="s">
+      <c r="B8" t="s">
         <v>169</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>170</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
oview updated by heike
</commit_message>
<xml_diff>
--- a/FSP_Exchange/data/Overview_Stat_Analyses.xlsx
+++ b/FSP_Exchange/data/Overview_Stat_Analyses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thermofisher-my.sharepoint.com/personal/heike_goehler_thermofisher_com/Documents/FSP_Exchange/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1016" documentId="8_{B71B119A-91B9-41B4-A31F-26ADBC8182F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8DCFF05-44FB-409F-875E-4CDB27F69245}"/>
+  <xr:revisionPtr revIDLastSave="1017" documentId="8_{B71B119A-91B9-41B4-A31F-26ADBC8182F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{944CF2D8-AB92-48D3-B891-93EDA9C6AA7E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{DB58F8A3-982D-4375-901B-E1B15CF4D99D}"/>
   </bookViews>
@@ -973,7 +973,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1286,7 +1286,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1362,7 +1362,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1661,13 +1661,13 @@
   <dimension ref="A1:AL137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="M8" sqref="M8"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" style="8" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" style="8" customWidth="1"/>
@@ -1696,7 +1696,7 @@
     <col min="25" max="26" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="22" customFormat="1">
+    <row r="1" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
@@ -1730,7 +1730,7 @@
       <c r="Y1" s="34"/>
       <c r="Z1" s="34"/>
     </row>
-    <row r="2" spans="1:26" s="22" customFormat="1">
+    <row r="2" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>3</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="26">
         <v>45334</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="26">
         <v>45334</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="26">
         <v>45334</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="26">
         <v>45334</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="26">
         <v>45334</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
         <v>45334</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="26">
         <v>45341</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="26">
         <v>45341</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="26">
         <v>45341</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
         <v>45341</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="26">
         <v>45341</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="27">
         <v>45341</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="26">
         <v>45334</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="26">
         <v>45334</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="26">
         <v>45334</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="27">
         <v>45334</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="26">
         <v>45334</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="26">
         <v>45334</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="26">
         <v>45334</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="26">
         <v>45334</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="26">
         <v>45334</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="26">
         <v>45334</v>
       </c>
@@ -3547,7 +3547,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="15.75" thickBot="1">
+    <row r="25" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="37">
         <v>45334</v>
       </c>
@@ -3626,7 +3626,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:26">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="26">
         <v>45343</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:26">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="27">
         <v>45343</v>
       </c>
@@ -3761,7 +3761,7 @@
         <v>35</v>
       </c>
       <c r="R27" s="29" t="s">
-        <v>35</v>
+        <v>112</v>
       </c>
       <c r="S27" s="15" t="s">
         <v>78</v>
@@ -3788,7 +3788,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:26">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="26">
         <v>45343</v>
       </c>
@@ -3869,7 +3869,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="29" spans="1:26">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="26">
         <v>45343</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="30" spans="1:26">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="26">
         <v>45343</v>
       </c>
@@ -4031,7 +4031,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="31" spans="1:26">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="26">
         <v>45343</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="32" spans="1:26">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="26">
         <v>45343</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="33" spans="1:26">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="26">
         <v>45343</v>
       </c>
@@ -4274,7 +4274,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="34" spans="1:26">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="26">
         <v>45343</v>
       </c>
@@ -4355,7 +4355,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="35" spans="1:26">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="26">
         <v>45343</v>
       </c>
@@ -4436,7 +4436,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="36" spans="1:26">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="26">
         <v>45343</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="37" spans="1:26">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="26">
         <v>45343</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:26">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="26">
         <v>45343</v>
       </c>
@@ -4679,7 +4679,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:26">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="26">
         <v>45343</v>
       </c>
@@ -4760,7 +4760,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:26">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="27">
         <v>45343</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:26">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="26">
         <v>45348</v>
       </c>
@@ -4922,7 +4922,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="42" spans="1:26">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="26">
         <v>45348</v>
       </c>
@@ -5003,7 +5003,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:26">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="26">
         <v>45348</v>
       </c>
@@ -5084,7 +5084,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="44" spans="1:26">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="26">
         <v>45348</v>
       </c>
@@ -5165,7 +5165,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:26">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="26">
         <v>45348</v>
       </c>
@@ -5246,7 +5246,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="46" spans="1:26">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="26">
         <v>45348</v>
       </c>
@@ -5327,7 +5327,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:26">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="26">
         <v>45348</v>
       </c>
@@ -5408,7 +5408,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="48" spans="1:26">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="26">
         <v>45348</v>
       </c>
@@ -5489,7 +5489,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:38">
+    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A49" s="26">
         <v>45348</v>
       </c>
@@ -5570,7 +5570,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="50" spans="1:38">
+    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A50" s="26">
         <v>45348</v>
       </c>
@@ -5651,7 +5651,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:38">
+    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A51" s="26">
         <v>45348</v>
       </c>
@@ -5732,7 +5732,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="52" spans="1:38">
+    <row r="52" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A52" s="26">
         <v>45348</v>
       </c>
@@ -5813,7 +5813,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="53" spans="1:38">
+    <row r="53" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A53" s="26">
         <v>45348</v>
       </c>
@@ -5894,7 +5894,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:38">
+    <row r="54" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A54" s="26">
         <v>45348</v>
       </c>
@@ -5975,7 +5975,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:38">
+    <row r="55" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A55" s="26">
         <v>45348</v>
       </c>
@@ -6056,7 +6056,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:38">
+    <row r="56" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A56" s="26">
         <v>45348</v>
       </c>
@@ -6137,7 +6137,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:38">
+    <row r="57" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A57" s="26">
         <v>45348</v>
       </c>
@@ -6218,7 +6218,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="58" spans="1:38">
+    <row r="58" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A58" s="26">
         <v>45348</v>
       </c>
@@ -6299,7 +6299,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="1:38">
+    <row r="59" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A59" s="26">
         <v>45348</v>
       </c>
@@ -6380,7 +6380,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="1:38">
+    <row r="60" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A60" s="26">
         <v>45348</v>
       </c>
@@ -6461,7 +6461,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="61" spans="1:38">
+    <row r="61" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A61" s="26">
         <v>45348</v>
       </c>
@@ -6542,7 +6542,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="62" spans="1:38">
+    <row r="62" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A62" s="26">
         <v>45348</v>
       </c>
@@ -6623,7 +6623,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="63" spans="1:38">
+    <row r="63" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A63" s="26">
         <v>45348</v>
       </c>
@@ -6705,7 +6705,7 @@
       </c>
       <c r="AL63" s="32"/>
     </row>
-    <row r="64" spans="1:38">
+    <row r="64" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A64" s="27">
         <v>45348</v>
       </c>
@@ -6787,7 +6787,7 @@
       </c>
       <c r="AL64" s="32"/>
     </row>
-    <row r="65" spans="1:26">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="26">
         <v>45356</v>
       </c>
@@ -6864,7 +6864,7 @@
       </c>
       <c r="Z65" s="18"/>
     </row>
-    <row r="66" spans="1:26">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="26">
         <v>45356</v>
       </c>
@@ -6941,7 +6941,7 @@
       </c>
       <c r="Z66" s="18"/>
     </row>
-    <row r="67" spans="1:26">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="26">
         <v>45356</v>
       </c>
@@ -7018,7 +7018,7 @@
       </c>
       <c r="Z67" s="18"/>
     </row>
-    <row r="68" spans="1:26">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="26">
         <v>45356</v>
       </c>
@@ -7095,7 +7095,7 @@
       </c>
       <c r="Z68" s="18"/>
     </row>
-    <row r="69" spans="1:26">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" s="26">
         <v>45356</v>
       </c>
@@ -7172,7 +7172,7 @@
       </c>
       <c r="Z69" s="18"/>
     </row>
-    <row r="70" spans="1:26">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" s="26">
         <v>45356</v>
       </c>
@@ -7249,7 +7249,7 @@
       </c>
       <c r="Z70" s="18"/>
     </row>
-    <row r="71" spans="1:26">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" s="26">
         <v>45356</v>
       </c>
@@ -7326,7 +7326,7 @@
       </c>
       <c r="Z71" s="18"/>
     </row>
-    <row r="72" spans="1:26">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" s="26">
         <v>45356</v>
       </c>
@@ -7403,7 +7403,7 @@
       </c>
       <c r="Z72" s="18"/>
     </row>
-    <row r="73" spans="1:26">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A73" s="26">
         <v>45356</v>
       </c>
@@ -7480,7 +7480,7 @@
       </c>
       <c r="Z73" s="18"/>
     </row>
-    <row r="74" spans="1:26">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A74" s="26">
         <v>45356</v>
       </c>
@@ -7557,7 +7557,7 @@
       </c>
       <c r="Z74" s="18"/>
     </row>
-    <row r="75" spans="1:26">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A75" s="26">
         <v>45356</v>
       </c>
@@ -7634,7 +7634,7 @@
       </c>
       <c r="Z75" s="18"/>
     </row>
-    <row r="76" spans="1:26">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A76" s="26">
         <v>45356</v>
       </c>
@@ -7711,7 +7711,7 @@
       </c>
       <c r="Z76" s="18"/>
     </row>
-    <row r="77" spans="1:26">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A77" s="26">
         <v>45356</v>
       </c>
@@ -7788,7 +7788,7 @@
       </c>
       <c r="Z77" s="18"/>
     </row>
-    <row r="78" spans="1:26">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A78" s="26">
         <v>45356</v>
       </c>
@@ -7865,7 +7865,7 @@
       </c>
       <c r="Z78" s="18"/>
     </row>
-    <row r="79" spans="1:26">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A79" s="26">
         <v>45356</v>
       </c>
@@ -7942,7 +7942,7 @@
       </c>
       <c r="Z79" s="18"/>
     </row>
-    <row r="80" spans="1:26">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A80" s="26">
         <v>45356</v>
       </c>
@@ -8019,7 +8019,7 @@
       </c>
       <c r="Z80" s="18"/>
     </row>
-    <row r="81" spans="1:26">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="26">
         <v>45356</v>
       </c>
@@ -8096,7 +8096,7 @@
       </c>
       <c r="Z81" s="18"/>
     </row>
-    <row r="82" spans="1:26">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" s="26">
         <v>45356</v>
       </c>
@@ -8173,7 +8173,7 @@
       </c>
       <c r="Z82" s="18"/>
     </row>
-    <row r="83" spans="1:26">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83" s="26">
         <v>45356</v>
       </c>
@@ -8250,7 +8250,7 @@
       </c>
       <c r="Z83" s="18"/>
     </row>
-    <row r="84" spans="1:26">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84" s="26">
         <v>45356</v>
       </c>
@@ -8327,7 +8327,7 @@
       </c>
       <c r="Z84" s="18"/>
     </row>
-    <row r="85" spans="1:26">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85" s="26">
         <v>45356</v>
       </c>
@@ -8404,7 +8404,7 @@
       </c>
       <c r="Z85" s="18"/>
     </row>
-    <row r="86" spans="1:26">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A86" s="26">
         <v>45356</v>
       </c>
@@ -8481,7 +8481,7 @@
       </c>
       <c r="Z86" s="18"/>
     </row>
-    <row r="87" spans="1:26">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" s="26">
         <v>45356</v>
       </c>
@@ -8558,7 +8558,7 @@
       </c>
       <c r="Z87" s="18"/>
     </row>
-    <row r="88" spans="1:26">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" s="26">
         <v>45356</v>
       </c>
@@ -8635,7 +8635,7 @@
       </c>
       <c r="Z88" s="18"/>
     </row>
-    <row r="89" spans="1:26">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A89" s="26">
         <v>45356</v>
       </c>
@@ -8712,7 +8712,7 @@
       </c>
       <c r="Z89" s="18"/>
     </row>
-    <row r="90" spans="1:26">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A90" s="26">
         <v>45356</v>
       </c>
@@ -8789,7 +8789,7 @@
       </c>
       <c r="Z90" s="18"/>
     </row>
-    <row r="91" spans="1:26">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A91" s="26">
         <v>45356</v>
       </c>
@@ -8866,7 +8866,7 @@
       </c>
       <c r="Z91" s="18"/>
     </row>
-    <row r="92" spans="1:26">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A92" s="26">
         <v>45356</v>
       </c>
@@ -8943,7 +8943,7 @@
       </c>
       <c r="Z92" s="18"/>
     </row>
-    <row r="93" spans="1:26">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A93" s="26">
         <v>45356</v>
       </c>
@@ -9020,7 +9020,7 @@
       </c>
       <c r="Z93" s="18"/>
     </row>
-    <row r="94" spans="1:26">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A94" s="26">
         <v>45356</v>
       </c>
@@ -9097,7 +9097,7 @@
       </c>
       <c r="Z94" s="18"/>
     </row>
-    <row r="95" spans="1:26">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A95" s="26">
         <v>45356</v>
       </c>
@@ -9174,7 +9174,7 @@
       </c>
       <c r="Z95" s="18"/>
     </row>
-    <row r="96" spans="1:26">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A96" s="26">
         <v>45356</v>
       </c>
@@ -9251,7 +9251,7 @@
       </c>
       <c r="Z96" s="18"/>
     </row>
-    <row r="97" spans="1:26">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A97" s="26">
         <v>45356</v>
       </c>
@@ -9328,7 +9328,7 @@
       </c>
       <c r="Z97" s="18"/>
     </row>
-    <row r="98" spans="1:26">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A98" s="26">
         <v>45356</v>
       </c>
@@ -9405,7 +9405,7 @@
       </c>
       <c r="Z98" s="18"/>
     </row>
-    <row r="99" spans="1:26">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A99" s="26">
         <v>45356</v>
       </c>
@@ -9482,7 +9482,7 @@
       </c>
       <c r="Z99" s="18"/>
     </row>
-    <row r="100" spans="1:26">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A100" s="26">
         <v>45356</v>
       </c>
@@ -9559,7 +9559,7 @@
       </c>
       <c r="Z100" s="18"/>
     </row>
-    <row r="101" spans="1:26">
+    <row r="101" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A101" s="26">
         <v>45356</v>
       </c>
@@ -9636,7 +9636,7 @@
       </c>
       <c r="Z101" s="18"/>
     </row>
-    <row r="102" spans="1:26">
+    <row r="102" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A102" s="26">
         <v>45356</v>
       </c>
@@ -9713,7 +9713,7 @@
       </c>
       <c r="Z102" s="18"/>
     </row>
-    <row r="103" spans="1:26">
+    <row r="103" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A103" s="26">
         <v>45356</v>
       </c>
@@ -9790,7 +9790,7 @@
       </c>
       <c r="Z103" s="18"/>
     </row>
-    <row r="104" spans="1:26">
+    <row r="104" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A104" s="26">
         <v>45356</v>
       </c>
@@ -9867,7 +9867,7 @@
       </c>
       <c r="Z104" s="18"/>
     </row>
-    <row r="105" spans="1:26">
+    <row r="105" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A105" s="26">
         <v>45356</v>
       </c>
@@ -9944,7 +9944,7 @@
       </c>
       <c r="Z105" s="18"/>
     </row>
-    <row r="106" spans="1:26">
+    <row r="106" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A106" s="26">
         <v>45356</v>
       </c>
@@ -10021,7 +10021,7 @@
       </c>
       <c r="Z106" s="18"/>
     </row>
-    <row r="107" spans="1:26">
+    <row r="107" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A107" s="26">
         <v>45356</v>
       </c>
@@ -10098,7 +10098,7 @@
       </c>
       <c r="Z107" s="18"/>
     </row>
-    <row r="108" spans="1:26">
+    <row r="108" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A108" s="26">
         <v>45356</v>
       </c>
@@ -10175,7 +10175,7 @@
       </c>
       <c r="Z108" s="18"/>
     </row>
-    <row r="109" spans="1:26">
+    <row r="109" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A109" s="26">
         <v>45356</v>
       </c>
@@ -10252,7 +10252,7 @@
       </c>
       <c r="Z109" s="18"/>
     </row>
-    <row r="110" spans="1:26">
+    <row r="110" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A110" s="26">
         <v>45356</v>
       </c>
@@ -10329,7 +10329,7 @@
       </c>
       <c r="Z110" s="18"/>
     </row>
-    <row r="111" spans="1:26">
+    <row r="111" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A111" s="26">
         <v>45356</v>
       </c>
@@ -10406,7 +10406,7 @@
       </c>
       <c r="Z111" s="18"/>
     </row>
-    <row r="112" spans="1:26">
+    <row r="112" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A112" s="26">
         <v>45356</v>
       </c>
@@ -10483,7 +10483,7 @@
       </c>
       <c r="Z112" s="18"/>
     </row>
-    <row r="113" spans="1:26">
+    <row r="113" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A113" s="26">
         <v>45356</v>
       </c>
@@ -10560,7 +10560,7 @@
       </c>
       <c r="Z113" s="18"/>
     </row>
-    <row r="114" spans="1:26">
+    <row r="114" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A114" s="26">
         <v>45356</v>
       </c>
@@ -10637,7 +10637,7 @@
       </c>
       <c r="Z114" s="18"/>
     </row>
-    <row r="115" spans="1:26">
+    <row r="115" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A115" s="26">
         <v>45356</v>
       </c>
@@ -10714,7 +10714,7 @@
       </c>
       <c r="Z115" s="18"/>
     </row>
-    <row r="116" spans="1:26">
+    <row r="116" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A116" s="26">
         <v>45356</v>
       </c>
@@ -10791,7 +10791,7 @@
       </c>
       <c r="Z116" s="18"/>
     </row>
-    <row r="117" spans="1:26">
+    <row r="117" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A117" s="26">
         <v>45356</v>
       </c>
@@ -10868,7 +10868,7 @@
       </c>
       <c r="Z117" s="18"/>
     </row>
-    <row r="118" spans="1:26">
+    <row r="118" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A118" s="26">
         <v>45356</v>
       </c>
@@ -10945,7 +10945,7 @@
       </c>
       <c r="Z118" s="18"/>
     </row>
-    <row r="119" spans="1:26">
+    <row r="119" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A119" s="26">
         <v>45356</v>
       </c>
@@ -11022,7 +11022,7 @@
       </c>
       <c r="Z119" s="18"/>
     </row>
-    <row r="120" spans="1:26">
+    <row r="120" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A120" s="27">
         <v>45356</v>
       </c>
@@ -11099,10 +11099,10 @@
       </c>
       <c r="Z120" s="14"/>
     </row>
-    <row r="136" spans="4:4">
+    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D136" s="1"/>
     </row>
-    <row r="137" spans="4:4">
+    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D137" s="1"/>
     </row>
   </sheetData>
@@ -11122,14 +11122,14 @@
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.28515625" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>291</v>
       </c>
@@ -11143,7 +11143,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>295</v>
       </c>
@@ -11157,7 +11157,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>298</v>
       </c>
@@ -11171,7 +11171,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>300</v>
       </c>
@@ -11185,7 +11185,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>302</v>
       </c>
@@ -11199,7 +11199,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>303</v>
       </c>
@@ -11213,7 +11213,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>305</v>
       </c>
@@ -11227,7 +11227,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>307</v>
       </c>
@@ -11241,7 +11241,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>309</v>
       </c>

</xml_diff>